<commit_message>
working on introduction...need more background info
</commit_message>
<xml_diff>
--- a/thesis1/data/litReviewTable.xlsx
+++ b/thesis1/data/litReviewTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/britanywuuu/Documents/ubc/Msc/hydrology/thesis1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{640EDD4B-9804-8643-ADB6-641E7B7BE1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971568EB-1908-1444-B893-44F9775DD556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{0CAAD55D-1984-2E4C-9A7E-557236EC3211}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{0CAAD55D-1984-2E4C-9A7E-557236EC3211}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Source</t>
   </si>
@@ -130,6 +130,87 @@
   </si>
   <si>
     <t xml:space="preserve">proportion of large landslides in forested areas is three time larger than non-forested in San Juan basin; no obvious trend found in between density and % logged. In the discussion, they mentioned logging accelerated mass wasting frequency but didn't infer where they got this conclusion from. </t>
+  </si>
+  <si>
+    <t>Keim and Skaugset, 2003</t>
+  </si>
+  <si>
+    <t>Pacific Northwest, USA</t>
+  </si>
+  <si>
+    <t>Use measured rainfall to simulate factor of safety under canopy vs no canopy scenario</t>
+  </si>
+  <si>
+    <t>peak intensities of throughfall is dampened and delayed under forest canopy; fos is bigger (less prone to landslide) in forested scenario</t>
+  </si>
+  <si>
+    <t>Bishop and Stevens</t>
+  </si>
+  <si>
+    <t>Southeast Alaska, USA</t>
+  </si>
+  <si>
+    <t>Assessed aerial photos, counted number and area of slides in each time period</t>
+  </si>
+  <si>
+    <t>number of landslides increased by 4.5 times within the 10 years after logging happened</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Lehmann et al., 2019</t>
+  </si>
+  <si>
+    <t>New Zealand, Oregon, Sumatra and Cambodia</t>
+  </si>
+  <si>
+    <t>Increased cumulative landslide area after deforestation (from 2 to 13 folds)</t>
+  </si>
+  <si>
+    <t>Use a hydro-mechanical andslide triggering model to simulate landslide frequency using remote sensing landcover data; based on threshold mechanics and progressive failure of hydrologically and mecchanically interacting soil columns. Use the greatest intensity rainfall within the triggering time frame to examine landslide activity before and after harvesting (they mentioned not just high intensity rainfall can trigger landslide)</t>
+  </si>
+  <si>
+    <t>Miller and Burnett, 2007</t>
+  </si>
+  <si>
+    <t>Oregon, USA</t>
+  </si>
+  <si>
+    <t>Logging and fire</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>FP??</t>
+  </si>
+  <si>
+    <t>Schmidt et al., 2001</t>
+  </si>
+  <si>
+    <t>Oregon Coast Range, USA</t>
+  </si>
+  <si>
+    <t>De Graff et al., 2012</t>
+  </si>
+  <si>
+    <t>Southern Thailand</t>
+  </si>
+  <si>
+    <t>Review of past landslide events and comparing the landslide triggering rain event; compare root strength of different vegetation type; compare % of landslide area in different land cover type</t>
+  </si>
+  <si>
+    <t>Focused on the importance of root strength in slope stability</t>
+  </si>
+  <si>
+    <t>Logging/conversion to rubber plantation</t>
+  </si>
+  <si>
+    <t>Investigated root strength in different forest covers. Compared root cohesion and landslide volume and perimeter in different forest types. Use field measurement of root strength to model slope stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landslides at clear-cut site higher -log(q/T), indicating low critical steady-state equivilant rainfall needed to trigger landslide;with similar root cohesion, landslidie initiating soil wetness was </t>
   </si>
 </sst>
 </file>
@@ -165,8 +246,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,21 +623,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEC95FB-3FC9-5540-8DF8-951C3FC99D05}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="97" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,8 +654,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -589,7 +675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -606,7 +692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -623,7 +709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -640,7 +726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -657,7 +743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -672,6 +758,105 @@
       </c>
       <c r="E7" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost done outline v2?
</commit_message>
<xml_diff>
--- a/thesis1/data/litReviewTable.xlsx
+++ b/thesis1/data/litReviewTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/britanywuuu/Documents/ubc/Msc/hydrology/thesis1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971568EB-1908-1444-B893-44F9775DD556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32882D9E-28F6-6146-8D8F-F5F27D8122A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{0CAAD55D-1984-2E4C-9A7E-557236EC3211}"/>
+    <workbookView xWindow="39320" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{0CAAD55D-1984-2E4C-9A7E-557236EC3211}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>Source</t>
   </si>
@@ -211,6 +211,18 @@
   </si>
   <si>
     <t xml:space="preserve">Landslides at clear-cut site higher -log(q/T), indicating low critical steady-state equivilant rainfall needed to trigger landslide;with similar root cohesion, landslidie initiating soil wetness was </t>
+  </si>
+  <si>
+    <t>Depicker et al., 2021</t>
+  </si>
+  <si>
+    <t>Kivu Rift, Africa (DRC, Rwanda and Burundi)</t>
+  </si>
+  <si>
+    <t>deforestation</t>
+  </si>
+  <si>
+    <t>Modelling</t>
   </si>
 </sst>
 </file>
@@ -623,10 +635,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEC95FB-3FC9-5540-8DF8-951C3FC99D05}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,6 +871,20 @@
         <v>54</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>